<commit_message>
(+)    small updates to plan
</commit_message>
<xml_diff>
--- a/Suppl/Thrive Fitness Plan - Lifting.xlsx
+++ b/Suppl/Thrive Fitness Plan - Lifting.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Day 1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="57">
   <si>
     <t>Day One</t>
   </si>
@@ -112,6 +112,87 @@
   </si>
   <si>
     <t>Dumbbell Lunge, Walking</t>
+  </si>
+  <si>
+    <t>3x15</t>
+  </si>
+  <si>
+    <t>3x10</t>
+  </si>
+  <si>
+    <t>3x12</t>
+  </si>
+  <si>
+    <t>3x8e</t>
+  </si>
+  <si>
+    <t>Lat Pulldown (slow negative)</t>
+  </si>
+  <si>
+    <t>T-ROW Machine</t>
+  </si>
+  <si>
+    <t>Standing Cable Bicep Curls</t>
+  </si>
+  <si>
+    <t>Seated DB Hammer Curls</t>
+  </si>
+  <si>
+    <t>Kettlebell Squat-to-Upright Row</t>
+  </si>
+  <si>
+    <t>Seated Back Extensions</t>
+  </si>
+  <si>
+    <t>Bent over Barbell Rows</t>
+  </si>
+  <si>
+    <t>Isometric Rear Delt Fly</t>
+  </si>
+  <si>
+    <t>4x60s</t>
+  </si>
+  <si>
+    <t>Low-to-High Side Chops (Kettlebell) 3x8e</t>
+  </si>
+  <si>
+    <t>Weighted Box Squats 3x10</t>
+  </si>
+  <si>
+    <t>Plank Hold 3x1min.</t>
+  </si>
+  <si>
+    <t>Medicine Ball Alt. Pushups 3x8e</t>
+  </si>
+  <si>
+    <t>Spiders (Knee to Elbow) 3x8e</t>
+  </si>
+  <si>
+    <t>Raised Leg Lifts 3x10</t>
+  </si>
+  <si>
+    <t>3x1min</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>(Bodyweight Plank)</t>
+  </si>
+  <si>
+    <t>(Raised Leg Lifts)</t>
+  </si>
+  <si>
+    <t>(Spiders, Knee to Elbow)</t>
+  </si>
+  <si>
+    <t>(Low-to-High Side Chops, Kettlebell)</t>
+  </si>
+  <si>
+    <t>(Dumbbell Squat, Assisted)</t>
+  </si>
+  <si>
+    <t>(Medicine Ball Pushup, Alternating)</t>
   </si>
 </sst>
 </file>
@@ -147,10 +228,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -507,7 +591,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -595,31 +679,175 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="38.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
(+)    Day Three Updates
</commit_message>
<xml_diff>
--- a/Suppl/Thrive Fitness Plan - Lifting.xlsx
+++ b/Suppl/Thrive Fitness Plan - Lifting.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Day 1" sheetId="1" r:id="rId1"/>
@@ -22,41 +22,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="62">
   <si>
     <t>Day One</t>
   </si>
   <si>
-    <t>● Incline DB Bench Press 3x10</t>
-  </si>
-  <si>
-    <t>● Pec-Dec Machine 3x12</t>
-  </si>
-  <si>
-    <t>● Standing Overhead Barbell Press 3x10</t>
-  </si>
-  <si>
-    <t>● Seated Single-Arm Tricep Extension 3x8e</t>
-  </si>
-  <si>
-    <t>● Bench Push-ups 3xFailure</t>
-  </si>
-  <si>
-    <t>● Squat to Press 3x10</t>
-  </si>
-  <si>
-    <t>● Rehab Focus:</t>
-  </si>
-  <si>
-    <t>○ Farmers Carry 3x20steps</t>
-  </si>
-  <si>
-    <t>Superset Rope Slams 3x1min.</t>
-  </si>
-  <si>
-    <t>SS</t>
-  </si>
-  <si>
     <t>Bodyweight Walking Lunges 3x15e</t>
   </si>
   <si>
@@ -120,79 +90,124 @@
     <t>3x10</t>
   </si>
   <si>
+    <t>3x8e</t>
+  </si>
+  <si>
+    <t>Low-to-High Side Chops (Kettlebell) 3x8e</t>
+  </si>
+  <si>
+    <t>Weighted Box Squats 3x10</t>
+  </si>
+  <si>
+    <t>Plank Hold 3x1min.</t>
+  </si>
+  <si>
+    <t>Medicine Ball Alt. Pushups 3x8e</t>
+  </si>
+  <si>
+    <t>Spiders (Knee to Elbow) 3x8e</t>
+  </si>
+  <si>
+    <t>Raised Leg Lifts 3x10</t>
+  </si>
+  <si>
+    <t>3x1min</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>(Bodyweight Plank)</t>
+  </si>
+  <si>
+    <t>(Raised Leg Lifts)</t>
+  </si>
+  <si>
+    <t>(Spiders, Knee to Elbow)</t>
+  </si>
+  <si>
+    <t>(Low-to-High Side Chops, Kettlebell)</t>
+  </si>
+  <si>
+    <t>(Dumbbell Squat, Assisted)</t>
+  </si>
+  <si>
+    <t>(Medicine Ball Pushup, Alternating)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T-ROW Machine </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seated DB Hammer Curls </t>
+  </si>
+  <si>
+    <t>3x8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Standing Cable Bicep Curls </t>
+  </si>
+  <si>
+    <t>3X12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bent over Barbell Rows </t>
+  </si>
+  <si>
+    <t>3x21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lat Pulldown (slow negative) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kettlebell Squat-to-Upright Row </t>
+  </si>
+  <si>
+    <t>Dips</t>
+  </si>
+  <si>
+    <t>Preacher Curls</t>
+  </si>
+  <si>
+    <t>Incline DB Press</t>
+  </si>
+  <si>
+    <t>Pec Deck Machine</t>
+  </si>
+  <si>
     <t>3x12</t>
   </si>
   <si>
-    <t>3x8e</t>
-  </si>
-  <si>
-    <t>Lat Pulldown (slow negative)</t>
-  </si>
-  <si>
-    <t>T-ROW Machine</t>
-  </si>
-  <si>
-    <t>Standing Cable Bicep Curls</t>
-  </si>
-  <si>
-    <t>Seated DB Hammer Curls</t>
-  </si>
-  <si>
-    <t>Kettlebell Squat-to-Upright Row</t>
-  </si>
-  <si>
-    <t>Seated Back Extensions</t>
-  </si>
-  <si>
-    <t>Bent over Barbell Rows</t>
-  </si>
-  <si>
-    <t>Isometric Rear Delt Fly</t>
-  </si>
-  <si>
-    <t>4x60s</t>
-  </si>
-  <si>
-    <t>Low-to-High Side Chops (Kettlebell) 3x8e</t>
-  </si>
-  <si>
-    <t>Weighted Box Squats 3x10</t>
-  </si>
-  <si>
-    <t>Plank Hold 3x1min.</t>
-  </si>
-  <si>
-    <t>Medicine Ball Alt. Pushups 3x8e</t>
-  </si>
-  <si>
-    <t>Spiders (Knee to Elbow) 3x8e</t>
-  </si>
-  <si>
-    <t>Raised Leg Lifts 3x10</t>
-  </si>
-  <si>
-    <t>3x1min</t>
-  </si>
-  <si>
-    <t>*</t>
-  </si>
-  <si>
-    <t>(Bodyweight Plank)</t>
-  </si>
-  <si>
-    <t>(Raised Leg Lifts)</t>
-  </si>
-  <si>
-    <t>(Spiders, Knee to Elbow)</t>
-  </si>
-  <si>
-    <t>(Low-to-High Side Chops, Kettlebell)</t>
-  </si>
-  <si>
-    <t>(Dumbbell Squat, Assisted)</t>
-  </si>
-  <si>
-    <t>(Medicine Ball Pushup, Alternating)</t>
+    <t>BB Shoulder Press</t>
+  </si>
+  <si>
+    <t>Farmer's Carry</t>
+  </si>
+  <si>
+    <t>3x60</t>
+  </si>
+  <si>
+    <t>DB Overhead Tricep Ext</t>
+  </si>
+  <si>
+    <t>Rope Slams</t>
+  </si>
+  <si>
+    <t>3x25</t>
+  </si>
+  <si>
+    <t>BW Pushups</t>
+  </si>
+  <si>
+    <t>DB Sq-Pr</t>
+  </si>
+  <si>
+    <t>3xFail</t>
+  </si>
+  <si>
+    <t>Iso Rear Delt Fly</t>
+  </si>
+  <si>
+    <t>3x60s</t>
   </si>
 </sst>
 </file>
@@ -228,14 +243,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -516,72 +533,92 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9:D10"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+      <c r="E2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="E3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+      <c r="E4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+      <c r="E5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+      <c r="E7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+      <c r="E8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+      <c r="E9" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" s="1"/>
+        <v>58</v>
+      </c>
+      <c r="E10" t="s">
+        <v>21</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="D9:D10"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
@@ -589,92 +626,93 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="37" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
         <v>11</v>
       </c>
-      <c r="C1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" t="s">
         <v>12</v>
       </c>
-      <c r="C2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" t="s">
         <v>13</v>
       </c>
-      <c r="C3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" t="s">
         <v>14</v>
       </c>
-      <c r="C4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" t="s">
         <v>15</v>
       </c>
-      <c r="C5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" t="s">
         <v>16</v>
       </c>
-      <c r="C6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" t="s">
         <v>18</v>
-      </c>
-      <c r="C8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" t="s">
-        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -685,77 +723,202 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>37</v>
-      </c>
-      <c r="E6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="B3" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="E7" t="s">
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>38</v>
-      </c>
-      <c r="E9" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>34</v>
-      </c>
-      <c r="E10" t="s">
-        <v>30</v>
-      </c>
+      <c r="B5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -763,7 +926,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -774,77 +937,77 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>33</v>
+        <v>23</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="C1" t="s">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D1" t="s">
-        <v>54</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>31</v>
+        <v>24</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="C2" t="s">
-        <v>55</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>49</v>
+        <v>25</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="C3" t="s">
-        <v>51</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>46</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>33</v>
+        <v>26</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="C4" t="s">
-        <v>56</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" t="s">
         <v>33</v>
-      </c>
-      <c r="C5" t="s">
-        <v>50</v>
-      </c>
-      <c r="D5" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>48</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="C6" t="s">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D6" t="s">
-        <v>52</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
(+)    completion of the Growth Phase plan!!
</commit_message>
<xml_diff>
--- a/Suppl/Thrive Fitness Plan - Lifting.xlsx
+++ b/Suppl/Thrive Fitness Plan - Lifting.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
-    <sheet name="Day 1" sheetId="1" r:id="rId1"/>
-    <sheet name="Day 2" sheetId="2" r:id="rId2"/>
-    <sheet name="Day 3" sheetId="3" r:id="rId3"/>
-    <sheet name="Day 4" sheetId="4" r:id="rId4"/>
+    <sheet name="Word Doc Sec" sheetId="5" r:id="rId1"/>
+    <sheet name="Day 1" sheetId="1" r:id="rId2"/>
+    <sheet name="Day 2" sheetId="2" r:id="rId3"/>
+    <sheet name="Day 3" sheetId="3" r:id="rId4"/>
+    <sheet name="Day 4" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="116">
   <si>
     <t>Day One</t>
   </si>
@@ -208,13 +209,175 @@
   </si>
   <si>
     <t>3x60s</t>
+  </si>
+  <si>
+    <t>Plan</t>
+  </si>
+  <si>
+    <t>Goal</t>
+  </si>
+  <si>
+    <t>Start</t>
+  </si>
+  <si>
+    <t>Style</t>
+  </si>
+  <si>
+    <t>Super-sets of two-lifts</t>
+  </si>
+  <si>
+    <t>Pre</t>
+  </si>
+  <si>
+    <t>10-15 min warm-up walk or run, 2 min gait train</t>
+  </si>
+  <si>
+    <t>Post</t>
+  </si>
+  <si>
+    <t>Day 1</t>
+  </si>
+  <si>
+    <t>Day 3</t>
+  </si>
+  <si>
+    <t>Day 2</t>
+  </si>
+  <si>
+    <t>Farmer's Carries</t>
+  </si>
+  <si>
+    <t>3x30</t>
+  </si>
+  <si>
+    <t>Day 4</t>
+  </si>
+  <si>
+    <t>4 day routine, rest every 7-14 days</t>
+  </si>
+  <si>
+    <t>15 min elliptical</t>
+  </si>
+  <si>
+    <t>Phase Two, Growth!</t>
+  </si>
+  <si>
+    <t>Functionality</t>
+  </si>
+  <si>
+    <t>Motion &amp; Control</t>
+  </si>
+  <si>
+    <t>Push</t>
+  </si>
+  <si>
+    <t>Lower</t>
+  </si>
+  <si>
+    <t>Focus on Control, on Symmetry</t>
+  </si>
+  <si>
+    <t>Pull</t>
+  </si>
+  <si>
+    <t>Inward Motion</t>
+  </si>
+  <si>
+    <t>Outward Motion</t>
+  </si>
+  <si>
+    <t>Dumbbell Incline Bench</t>
+  </si>
+  <si>
+    <t>Pec-Deck Machine</t>
+  </si>
+  <si>
+    <t>Barbbell Shoulder Press, Military</t>
+  </si>
+  <si>
+    <t>Isometric Rear Delt Fly</t>
+  </si>
+  <si>
+    <t>Seated Dumbbell Tricep Overhead Extension</t>
+  </si>
+  <si>
+    <t>Bench Pushups</t>
+  </si>
+  <si>
+    <t>Dumbbell Squat-to-Press</t>
+  </si>
+  <si>
+    <t>Machine Individual Leg Press</t>
+  </si>
+  <si>
+    <t>Dumbbell Lunges</t>
+  </si>
+  <si>
+    <t>Seated Lower Back Extension</t>
+  </si>
+  <si>
+    <t>Rope Pulls</t>
+  </si>
+  <si>
+    <t>Bosu Ball Dumbbell Squats</t>
+  </si>
+  <si>
+    <t>Russian Twist w/Medicine Ball</t>
+  </si>
+  <si>
+    <t>Calf Raises</t>
+  </si>
+  <si>
+    <t>T-ROW Machine</t>
+  </si>
+  <si>
+    <t>Dumbbell Curls</t>
+  </si>
+  <si>
+    <t>Bent-over Barbbell Row</t>
+  </si>
+  <si>
+    <t>Dumbbell Hammer Curls</t>
+  </si>
+  <si>
+    <t>Dumbbell Preacher Curl 21's</t>
+  </si>
+  <si>
+    <t>Lateral Pulldown, slow-release</t>
+  </si>
+  <si>
+    <t>Kettlebell Squat-to-Upright Row</t>
+  </si>
+  <si>
+    <t>TRX Single-Leg Squats</t>
+  </si>
+  <si>
+    <t>Low-to-High Kettlebell Side-Chops</t>
+  </si>
+  <si>
+    <t>Dumbbelll Squats to Box</t>
+  </si>
+  <si>
+    <t>TRX Rows</t>
+  </si>
+  <si>
+    <t>Planks</t>
+  </si>
+  <si>
+    <t>Medicine Ball Pushups (alt)</t>
+  </si>
+  <si>
+    <t>Spider Crawls, Knee-to-Elbow</t>
+  </si>
+  <si>
+    <t>Raised Leg Lifts</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -222,16 +385,75 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -239,11 +461,48 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -253,6 +512,51 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -533,6 +837,761 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L40"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I36" sqref="I36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="22.7109375" customWidth="1"/>
+    <col min="260" max="260" width="19.85546875" customWidth="1"/>
+    <col min="516" max="516" width="19.85546875" customWidth="1"/>
+    <col min="772" max="772" width="19.85546875" customWidth="1"/>
+    <col min="1028" max="1028" width="19.85546875" customWidth="1"/>
+    <col min="1284" max="1284" width="19.85546875" customWidth="1"/>
+    <col min="1540" max="1540" width="19.85546875" customWidth="1"/>
+    <col min="1796" max="1796" width="19.85546875" customWidth="1"/>
+    <col min="2052" max="2052" width="19.85546875" customWidth="1"/>
+    <col min="2308" max="2308" width="19.85546875" customWidth="1"/>
+    <col min="2564" max="2564" width="19.85546875" customWidth="1"/>
+    <col min="2820" max="2820" width="19.85546875" customWidth="1"/>
+    <col min="3076" max="3076" width="19.85546875" customWidth="1"/>
+    <col min="3332" max="3332" width="19.85546875" customWidth="1"/>
+    <col min="3588" max="3588" width="19.85546875" customWidth="1"/>
+    <col min="3844" max="3844" width="19.85546875" customWidth="1"/>
+    <col min="4100" max="4100" width="19.85546875" customWidth="1"/>
+    <col min="4356" max="4356" width="19.85546875" customWidth="1"/>
+    <col min="4612" max="4612" width="19.85546875" customWidth="1"/>
+    <col min="4868" max="4868" width="19.85546875" customWidth="1"/>
+    <col min="5124" max="5124" width="19.85546875" customWidth="1"/>
+    <col min="5380" max="5380" width="19.85546875" customWidth="1"/>
+    <col min="5636" max="5636" width="19.85546875" customWidth="1"/>
+    <col min="5892" max="5892" width="19.85546875" customWidth="1"/>
+    <col min="6148" max="6148" width="19.85546875" customWidth="1"/>
+    <col min="6404" max="6404" width="19.85546875" customWidth="1"/>
+    <col min="6660" max="6660" width="19.85546875" customWidth="1"/>
+    <col min="6916" max="6916" width="19.85546875" customWidth="1"/>
+    <col min="7172" max="7172" width="19.85546875" customWidth="1"/>
+    <col min="7428" max="7428" width="19.85546875" customWidth="1"/>
+    <col min="7684" max="7684" width="19.85546875" customWidth="1"/>
+    <col min="7940" max="7940" width="19.85546875" customWidth="1"/>
+    <col min="8196" max="8196" width="19.85546875" customWidth="1"/>
+    <col min="8452" max="8452" width="19.85546875" customWidth="1"/>
+    <col min="8708" max="8708" width="19.85546875" customWidth="1"/>
+    <col min="8964" max="8964" width="19.85546875" customWidth="1"/>
+    <col min="9220" max="9220" width="19.85546875" customWidth="1"/>
+    <col min="9476" max="9476" width="19.85546875" customWidth="1"/>
+    <col min="9732" max="9732" width="19.85546875" customWidth="1"/>
+    <col min="9988" max="9988" width="19.85546875" customWidth="1"/>
+    <col min="10244" max="10244" width="19.85546875" customWidth="1"/>
+    <col min="10500" max="10500" width="19.85546875" customWidth="1"/>
+    <col min="10756" max="10756" width="19.85546875" customWidth="1"/>
+    <col min="11012" max="11012" width="19.85546875" customWidth="1"/>
+    <col min="11268" max="11268" width="19.85546875" customWidth="1"/>
+    <col min="11524" max="11524" width="19.85546875" customWidth="1"/>
+    <col min="11780" max="11780" width="19.85546875" customWidth="1"/>
+    <col min="12036" max="12036" width="19.85546875" customWidth="1"/>
+    <col min="12292" max="12292" width="19.85546875" customWidth="1"/>
+    <col min="12548" max="12548" width="19.85546875" customWidth="1"/>
+    <col min="12804" max="12804" width="19.85546875" customWidth="1"/>
+    <col min="13060" max="13060" width="19.85546875" customWidth="1"/>
+    <col min="13316" max="13316" width="19.85546875" customWidth="1"/>
+    <col min="13572" max="13572" width="19.85546875" customWidth="1"/>
+    <col min="13828" max="13828" width="19.85546875" customWidth="1"/>
+    <col min="14084" max="14084" width="19.85546875" customWidth="1"/>
+    <col min="14340" max="14340" width="19.85546875" customWidth="1"/>
+    <col min="14596" max="14596" width="19.85546875" customWidth="1"/>
+    <col min="14852" max="14852" width="19.85546875" customWidth="1"/>
+    <col min="15108" max="15108" width="19.85546875" customWidth="1"/>
+    <col min="15364" max="15364" width="19.85546875" customWidth="1"/>
+    <col min="15620" max="15620" width="19.85546875" customWidth="1"/>
+    <col min="15876" max="15876" width="19.85546875" customWidth="1"/>
+    <col min="16132" max="16132" width="19.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+    </row>
+    <row r="2" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" s="24">
+        <v>42767</v>
+      </c>
+      <c r="C2" s="24"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+    </row>
+    <row r="3" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+    </row>
+    <row r="4" spans="1:11" ht="6.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+    </row>
+    <row r="5" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="F5" s="13"/>
+      <c r="G5" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="12" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="14"/>
+      <c r="B6" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="C6" s="25"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="15"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="I6" s="17"/>
+      <c r="J6" s="17"/>
+      <c r="K6" s="27" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="14"/>
+      <c r="B7" s="25" t="s">
+        <v>88</v>
+      </c>
+      <c r="C7" s="25"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="F7" s="15"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="I7" s="17"/>
+      <c r="J7" s="17"/>
+      <c r="K7" s="27" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="14"/>
+      <c r="B8" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="C8" s="25"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" s="15"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="I8" s="17"/>
+      <c r="J8" s="17"/>
+      <c r="K8" s="27" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="14"/>
+      <c r="B9" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="C9" s="25"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="F9" s="15"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="I9" s="17"/>
+      <c r="J9" s="17"/>
+      <c r="K9" s="27" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="14"/>
+      <c r="B10" s="25" t="s">
+        <v>90</v>
+      </c>
+      <c r="C10" s="25"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="26" t="s">
+        <v>61</v>
+      </c>
+      <c r="F10" s="13"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="I10" s="17"/>
+      <c r="J10" s="17"/>
+      <c r="K10" s="27" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="14"/>
+      <c r="B11" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="C11" s="25"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="F11" s="15"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="I11" s="17"/>
+      <c r="J11" s="17"/>
+      <c r="K11" s="27" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="14"/>
+      <c r="B12" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="C12" s="25"/>
+      <c r="D12" s="25"/>
+      <c r="E12" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="F12" s="15"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="17" t="s">
+        <v>106</v>
+      </c>
+      <c r="I12" s="17"/>
+      <c r="J12" s="17"/>
+      <c r="K12" s="27" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="14"/>
+      <c r="B13" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="C13" s="25"/>
+      <c r="D13" s="25"/>
+      <c r="E13" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="F13" s="15"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="I13" s="17"/>
+      <c r="J13" s="17"/>
+      <c r="K13" s="27" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="14"/>
+      <c r="B14" s="25" t="s">
+        <v>93</v>
+      </c>
+      <c r="C14" s="25"/>
+      <c r="D14" s="25"/>
+      <c r="E14" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="F14" s="15"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="6"/>
+    </row>
+    <row r="15" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="5"/>
+      <c r="B15" s="18"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="H15" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="I15" s="21"/>
+      <c r="J15" s="21"/>
+      <c r="K15" s="12" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" s="6" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="F16" s="15"/>
+      <c r="G16" s="22"/>
+      <c r="H16" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="I16" s="23"/>
+      <c r="J16" s="23"/>
+      <c r="K16" s="28" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="19"/>
+      <c r="B17" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="C17" s="20"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="F17" s="9"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="23" t="s">
+        <v>109</v>
+      </c>
+      <c r="I17" s="23"/>
+      <c r="J17" s="23"/>
+      <c r="K17" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="L17" s="6"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="19"/>
+      <c r="B18" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="C18" s="20"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="F18" s="9"/>
+      <c r="G18" s="22"/>
+      <c r="H18" s="23" t="s">
+        <v>110</v>
+      </c>
+      <c r="I18" s="23"/>
+      <c r="J18" s="23"/>
+      <c r="K18" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="L18" s="6"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="19"/>
+      <c r="B19" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" s="20"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="F19" s="6"/>
+      <c r="G19" s="22"/>
+      <c r="H19" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="I19" s="23"/>
+      <c r="J19" s="23"/>
+      <c r="K19" s="28" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="19"/>
+      <c r="B20" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="C20" s="20"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="F20" s="6"/>
+      <c r="G20" s="22"/>
+      <c r="H20" s="23" t="s">
+        <v>112</v>
+      </c>
+      <c r="I20" s="23"/>
+      <c r="J20" s="23"/>
+      <c r="K20" s="28" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="19"/>
+      <c r="B21" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="C21" s="20"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="F21" s="6"/>
+      <c r="G21" s="22"/>
+      <c r="H21" s="23" t="s">
+        <v>113</v>
+      </c>
+      <c r="I21" s="23"/>
+      <c r="J21" s="23"/>
+      <c r="K21" s="28" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="19"/>
+      <c r="B22" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="C22" s="20"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="F22" s="6"/>
+      <c r="G22" s="22"/>
+      <c r="H22" s="23" t="s">
+        <v>114</v>
+      </c>
+      <c r="I22" s="23"/>
+      <c r="J22" s="23"/>
+      <c r="K22" s="28" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" s="19"/>
+      <c r="B23" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" s="20"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="F23" s="6"/>
+      <c r="G23" s="22"/>
+      <c r="H23" s="23" t="s">
+        <v>115</v>
+      </c>
+      <c r="I23" s="23"/>
+      <c r="J23" s="23"/>
+      <c r="K23" s="28" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" s="19"/>
+      <c r="B24" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="C24" s="20"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="6"/>
+      <c r="K24" s="6"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" s="19"/>
+      <c r="B25" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="C25" s="20"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
+      <c r="I25" s="6"/>
+      <c r="J25" s="6"/>
+      <c r="K25" s="6"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" s="19"/>
+      <c r="B26" s="20" t="s">
+        <v>100</v>
+      </c>
+      <c r="C26" s="20"/>
+      <c r="D26" s="20"/>
+      <c r="E26" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="6"/>
+      <c r="J26" s="6"/>
+      <c r="K26" s="6"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" s="6"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="6"/>
+      <c r="I27" s="6"/>
+      <c r="J27" s="6"/>
+      <c r="K27" s="6"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" s="6"/>
+      <c r="B28" s="6"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="6"/>
+      <c r="H28" s="6"/>
+      <c r="I28" s="6"/>
+      <c r="J28" s="6"/>
+      <c r="K28" s="6"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" s="6"/>
+      <c r="B29" s="6"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="6"/>
+      <c r="I29" s="6"/>
+      <c r="J29" s="6"/>
+      <c r="K29" s="6"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" s="6"/>
+      <c r="B30" s="6"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="6"/>
+      <c r="H30" s="6"/>
+      <c r="I30" s="6"/>
+      <c r="J30" s="6"/>
+      <c r="K30" s="6"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" s="6"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="6"/>
+      <c r="H31" s="6"/>
+      <c r="I31" s="6"/>
+      <c r="J31" s="6"/>
+      <c r="K31" s="6"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32" s="6"/>
+      <c r="B32" s="6"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="6"/>
+      <c r="G32" s="6"/>
+      <c r="H32" s="6"/>
+      <c r="I32" s="6"/>
+      <c r="J32" s="6"/>
+      <c r="K32" s="6"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="6"/>
+      <c r="B33" s="6"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="6"/>
+      <c r="B34" s="6"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="6"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="6"/>
+      <c r="B35" s="6"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="6"/>
+      <c r="F35" s="6"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="6"/>
+      <c r="B36" s="6"/>
+      <c r="C36" s="6"/>
+      <c r="D36" s="6"/>
+      <c r="E36" s="6"/>
+      <c r="F36" s="6"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="6"/>
+      <c r="B37" s="6"/>
+      <c r="C37" s="6"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="6"/>
+      <c r="F37" s="6"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="6"/>
+      <c r="B38" s="6"/>
+      <c r="C38" s="6"/>
+      <c r="D38" s="6"/>
+      <c r="E38" s="6"/>
+      <c r="F38" s="6"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="6"/>
+      <c r="B39" s="6"/>
+      <c r="C39" s="6"/>
+      <c r="D39" s="6"/>
+      <c r="E39" s="6"/>
+      <c r="F39" s="6"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="6"/>
+      <c r="B40" s="6"/>
+      <c r="C40" s="6"/>
+      <c r="D40" s="6"/>
+      <c r="E40" s="6"/>
+      <c r="F40" s="6"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:C2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -624,11 +1683,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
@@ -721,7 +1780,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H15"/>
   <sheetViews>
@@ -922,7 +1981,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D6"/>
   <sheetViews>

</xml_diff>

<commit_message>
(+)    added Caitlin's new diet plans
</commit_message>
<xml_diff>
--- a/Suppl/Thrive Fitness Plan - Lifting.xlsx
+++ b/Suppl/Thrive Fitness Plan - Lifting.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="115">
   <si>
     <t>Day One</t>
   </si>
@@ -145,12 +145,6 @@
     <t>3x8</t>
   </si>
   <si>
-    <t xml:space="preserve">Standing Cable Bicep Curls </t>
-  </si>
-  <si>
-    <t>3X12</t>
-  </si>
-  <si>
     <t xml:space="preserve">Bent over Barbell Rows </t>
   </si>
   <si>
@@ -331,15 +325,9 @@
     <t>T-ROW Machine</t>
   </si>
   <si>
-    <t>Dumbbell Curls</t>
-  </si>
-  <si>
     <t>Bent-over Barbbell Row</t>
   </si>
   <si>
-    <t>Dumbbell Hammer Curls</t>
-  </si>
-  <si>
     <t>Dumbbell Preacher Curl 21's</t>
   </si>
   <si>
@@ -371,6 +359,15 @@
   </si>
   <si>
     <t>Raised Leg Lifts</t>
+  </si>
+  <si>
+    <t>Barbeell Curls</t>
+  </si>
+  <si>
+    <t>Barbbell Curls</t>
+  </si>
+  <si>
+    <t>Seated Dumbbell Hammer Curls</t>
   </si>
 </sst>
 </file>
@@ -409,7 +406,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -449,6 +446,30 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -502,7 +523,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -541,9 +562,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -557,6 +575,13 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -840,12 +865,14 @@
   <dimension ref="A1:L40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I36" sqref="I36"/>
+      <selection activeCell="AG5" sqref="AG5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="22.7109375" customWidth="1"/>
+    <col min="10" max="10" width="18.28515625" customWidth="1"/>
+    <col min="11" max="11" width="5.5703125" customWidth="1"/>
     <col min="260" max="260" width="19.85546875" customWidth="1"/>
     <col min="516" max="516" width="19.85546875" customWidth="1"/>
     <col min="772" max="772" width="19.85546875" customWidth="1"/>
@@ -911,70 +938,70 @@
     <col min="16132" max="16132" width="19.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C1" s="5"/>
       <c r="D1" s="5"/>
       <c r="E1" s="7"/>
       <c r="F1" s="7"/>
       <c r="G1" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I1" s="6"/>
       <c r="J1" s="6"/>
       <c r="K1" s="6"/>
     </row>
-    <row r="2" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="B2" s="24">
+        <v>62</v>
+      </c>
+      <c r="B2" s="29">
         <v>42767</v>
       </c>
-      <c r="C2" s="24"/>
+      <c r="C2" s="29"/>
       <c r="D2" s="5"/>
       <c r="E2" s="7"/>
       <c r="F2" s="7"/>
       <c r="G2" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I2" s="6"/>
       <c r="J2" s="6"/>
       <c r="K2" s="6"/>
     </row>
-    <row r="3" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
       <c r="G3" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="I3" s="6"/>
       <c r="J3" s="6"/>
       <c r="K3" s="6"/>
     </row>
-    <row r="4" spans="1:11" ht="6.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="6.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6"/>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
@@ -987,207 +1014,207 @@
       <c r="J4" s="6"/>
       <c r="K4" s="6"/>
     </row>
-    <row r="5" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="10" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
       <c r="E5" s="12" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F5" s="13"/>
       <c r="G5" s="10" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H5" s="11" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="I5" s="11"/>
       <c r="J5" s="11"/>
       <c r="K5" s="12" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="33"/>
+      <c r="B6" s="24" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="14"/>
-      <c r="B6" s="25" t="s">
-        <v>87</v>
-      </c>
-      <c r="C6" s="25"/>
-      <c r="D6" s="25"/>
-      <c r="E6" s="26" t="s">
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="25" t="s">
         <v>21</v>
       </c>
       <c r="F6" s="15"/>
-      <c r="G6" s="16"/>
+      <c r="G6" s="30"/>
       <c r="H6" s="17" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="I6" s="17"/>
       <c r="J6" s="17"/>
-      <c r="K6" s="27" t="s">
+      <c r="K6" s="26" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="14"/>
-      <c r="B7" s="25" t="s">
-        <v>88</v>
-      </c>
-      <c r="C7" s="25"/>
-      <c r="D7" s="25"/>
-      <c r="E7" s="26" t="s">
-        <v>50</v>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="33"/>
+      <c r="B7" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="C7" s="24"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="25" t="s">
+        <v>48</v>
       </c>
       <c r="F7" s="15"/>
-      <c r="G7" s="16"/>
+      <c r="G7" s="30"/>
       <c r="H7" s="17" t="s">
-        <v>102</v>
+        <v>112</v>
       </c>
       <c r="I7" s="17"/>
       <c r="J7" s="17"/>
-      <c r="K7" s="27" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K7" s="26" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="14"/>
-      <c r="B8" s="25" t="s">
-        <v>89</v>
-      </c>
-      <c r="C8" s="25"/>
-      <c r="D8" s="25"/>
-      <c r="E8" s="26" t="s">
+      <c r="B8" s="24" t="s">
+        <v>87</v>
+      </c>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="25" t="s">
         <v>21</v>
       </c>
       <c r="F8" s="15"/>
       <c r="G8" s="16"/>
       <c r="H8" s="17" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="I8" s="17"/>
       <c r="J8" s="17"/>
-      <c r="K8" s="27" t="s">
+      <c r="K8" s="26" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="14"/>
-      <c r="B9" s="25" t="s">
-        <v>73</v>
-      </c>
-      <c r="C9" s="25"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="26" t="s">
-        <v>53</v>
+      <c r="B9" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="C9" s="24"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="25" t="s">
+        <v>51</v>
       </c>
       <c r="F9" s="15"/>
       <c r="G9" s="16"/>
       <c r="H9" s="17" t="s">
-        <v>104</v>
+        <v>114</v>
       </c>
       <c r="I9" s="17"/>
       <c r="J9" s="17"/>
-      <c r="K9" s="27" t="s">
+      <c r="K9" s="26" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="14"/>
-      <c r="B10" s="25" t="s">
-        <v>90</v>
-      </c>
-      <c r="C10" s="25"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="26" t="s">
-        <v>61</v>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="33"/>
+      <c r="B10" s="24" t="s">
+        <v>88</v>
+      </c>
+      <c r="C10" s="24"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="25" t="s">
+        <v>59</v>
       </c>
       <c r="F10" s="13"/>
-      <c r="G10" s="16"/>
+      <c r="G10" s="30"/>
       <c r="H10" s="17" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="I10" s="17"/>
       <c r="J10" s="17"/>
-      <c r="K10" s="27" t="s">
+      <c r="K10" s="26" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="14"/>
-      <c r="B11" s="25" t="s">
-        <v>91</v>
-      </c>
-      <c r="C11" s="25"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="26" t="s">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="33"/>
+      <c r="B11" s="24" t="s">
+        <v>89</v>
+      </c>
+      <c r="C11" s="24"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="25" t="s">
         <v>39</v>
       </c>
       <c r="F11" s="15"/>
-      <c r="G11" s="16"/>
+      <c r="G11" s="30"/>
       <c r="H11" s="17" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="I11" s="17"/>
       <c r="J11" s="17"/>
-      <c r="K11" s="27" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K11" s="26" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="14"/>
-      <c r="B12" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="C12" s="25"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="26" t="s">
-        <v>56</v>
+      <c r="B12" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" s="24"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="25" t="s">
+        <v>54</v>
       </c>
       <c r="F12" s="15"/>
       <c r="G12" s="16"/>
       <c r="H12" s="17" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="I12" s="17"/>
       <c r="J12" s="17"/>
-      <c r="K12" s="27" t="s">
+      <c r="K12" s="26" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="14"/>
-      <c r="B13" s="25" t="s">
-        <v>92</v>
-      </c>
-      <c r="C13" s="25"/>
-      <c r="D13" s="25"/>
-      <c r="E13" s="26" t="s">
-        <v>59</v>
+      <c r="B13" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="C13" s="24"/>
+      <c r="D13" s="24"/>
+      <c r="E13" s="25" t="s">
+        <v>57</v>
       </c>
       <c r="F13" s="15"/>
       <c r="G13" s="16"/>
       <c r="H13" s="17" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="I13" s="17"/>
       <c r="J13" s="17"/>
-      <c r="K13" s="27" t="s">
+      <c r="K13" s="26" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="14"/>
-      <c r="B14" s="25" t="s">
-        <v>93</v>
-      </c>
-      <c r="C14" s="25"/>
-      <c r="D14" s="25"/>
-      <c r="E14" s="26" t="s">
+      <c r="B14" s="24" t="s">
+        <v>91</v>
+      </c>
+      <c r="C14" s="24"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="25" t="s">
         <v>21</v>
       </c>
       <c r="F14" s="15"/>
@@ -1197,7 +1224,7 @@
       <c r="J14" s="6"/>
       <c r="K14" s="6"/>
     </row>
-    <row r="15" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="5"/>
       <c r="B15" s="18"/>
       <c r="C15" s="6"/>
@@ -1205,83 +1232,83 @@
       <c r="E15" s="15"/>
       <c r="F15" s="15"/>
       <c r="G15" s="10" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="H15" s="11" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="I15" s="21"/>
       <c r="J15" s="21"/>
       <c r="K15" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="L15" s="6"/>
+    </row>
+    <row r="16" spans="1:12" s="6" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="B16" s="11" t="s">
         <v>80</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" s="6" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="B16" s="11" t="s">
-        <v>82</v>
       </c>
       <c r="C16" s="11"/>
       <c r="D16" s="11"/>
       <c r="E16" s="12" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F16" s="15"/>
-      <c r="G16" s="22"/>
+      <c r="G16" s="32"/>
       <c r="H16" s="23" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="I16" s="23"/>
       <c r="J16" s="23"/>
-      <c r="K16" s="28" t="s">
+      <c r="K16" s="27" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="19"/>
+      <c r="A17" s="31"/>
       <c r="B17" s="20" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C17" s="20"/>
       <c r="D17" s="20"/>
-      <c r="E17" s="29" t="s">
+      <c r="E17" s="28" t="s">
         <v>39</v>
       </c>
       <c r="F17" s="9"/>
-      <c r="G17" s="22"/>
+      <c r="G17" s="32"/>
       <c r="H17" s="23" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="I17" s="23"/>
       <c r="J17" s="23"/>
-      <c r="K17" s="28" t="s">
+      <c r="K17" s="27" t="s">
         <v>39</v>
       </c>
       <c r="L17" s="6"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="19"/>
+      <c r="A18" s="31"/>
       <c r="B18" s="20" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C18" s="20"/>
       <c r="D18" s="20"/>
-      <c r="E18" s="29" t="s">
-        <v>74</v>
+      <c r="E18" s="28" t="s">
+        <v>72</v>
       </c>
       <c r="F18" s="9"/>
       <c r="G18" s="22"/>
       <c r="H18" s="23" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="I18" s="23"/>
       <c r="J18" s="23"/>
-      <c r="K18" s="28" t="s">
+      <c r="K18" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="L18" s="6"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="19"/>
@@ -1290,112 +1317,112 @@
       </c>
       <c r="C19" s="20"/>
       <c r="D19" s="20"/>
-      <c r="E19" s="29" t="s">
+      <c r="E19" s="28" t="s">
         <v>21</v>
       </c>
       <c r="F19" s="6"/>
       <c r="G19" s="22"/>
       <c r="H19" s="23" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="I19" s="23"/>
       <c r="J19" s="23"/>
-      <c r="K19" s="28" t="s">
-        <v>50</v>
+      <c r="K19" s="27" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="19"/>
       <c r="B20" s="20" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C20" s="20"/>
       <c r="D20" s="20"/>
-      <c r="E20" s="29" t="s">
-        <v>50</v>
+      <c r="E20" s="28" t="s">
+        <v>48</v>
       </c>
       <c r="F20" s="6"/>
       <c r="G20" s="22"/>
       <c r="H20" s="23" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="I20" s="23"/>
       <c r="J20" s="23"/>
-      <c r="K20" s="28" t="s">
-        <v>61</v>
+      <c r="K20" s="27" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="19"/>
+      <c r="A21" s="31"/>
       <c r="B21" s="20" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C21" s="20"/>
       <c r="D21" s="20"/>
-      <c r="E21" s="29" t="s">
-        <v>61</v>
+      <c r="E21" s="28" t="s">
+        <v>59</v>
       </c>
       <c r="F21" s="6"/>
-      <c r="G21" s="22"/>
+      <c r="G21" s="32"/>
       <c r="H21" s="23" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="I21" s="23"/>
       <c r="J21" s="23"/>
-      <c r="K21" s="28" t="s">
+      <c r="K21" s="27" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="19"/>
+      <c r="A22" s="31"/>
       <c r="B22" s="20" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C22" s="20"/>
       <c r="D22" s="20"/>
-      <c r="E22" s="29" t="s">
+      <c r="E22" s="28" t="s">
         <v>21</v>
       </c>
       <c r="F22" s="6"/>
-      <c r="G22" s="22"/>
+      <c r="G22" s="32"/>
       <c r="H22" s="23" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="I22" s="23"/>
       <c r="J22" s="23"/>
-      <c r="K22" s="28" t="s">
+      <c r="K22" s="27" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="19"/>
+      <c r="A23" s="31"/>
       <c r="B23" s="20" t="s">
         <v>14</v>
       </c>
       <c r="C23" s="20"/>
       <c r="D23" s="20"/>
-      <c r="E23" s="29" t="s">
+      <c r="E23" s="28" t="s">
         <v>20</v>
       </c>
       <c r="F23" s="6"/>
-      <c r="G23" s="22"/>
+      <c r="G23" s="32"/>
       <c r="H23" s="23" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="I23" s="23"/>
       <c r="J23" s="23"/>
-      <c r="K23" s="28" t="s">
+      <c r="K23" s="27" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="19"/>
       <c r="B24" s="20" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C24" s="20"/>
       <c r="D24" s="20"/>
-      <c r="E24" s="29" t="s">
+      <c r="E24" s="28" t="s">
         <v>21</v>
       </c>
       <c r="F24" s="6"/>
@@ -1412,7 +1439,7 @@
       </c>
       <c r="C25" s="20"/>
       <c r="D25" s="20"/>
-      <c r="E25" s="29" t="s">
+      <c r="E25" s="28" t="s">
         <v>20</v>
       </c>
       <c r="F25" s="6"/>
@@ -1425,11 +1452,11 @@
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="19"/>
       <c r="B26" s="20" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C26" s="20"/>
       <c r="D26" s="20"/>
-      <c r="E26" s="29" t="s">
+      <c r="E26" s="28" t="s">
         <v>20</v>
       </c>
       <c r="F26" s="6"/>
@@ -1595,7 +1622,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="C58" sqref="C58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1607,7 +1634,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E2" t="s">
         <v>21</v>
@@ -1615,15 +1642,15 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E4" t="s">
         <v>21</v>
@@ -1631,23 +1658,23 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E7" t="s">
         <v>39</v>
@@ -1655,23 +1682,23 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>55</v>
+      </c>
+      <c r="E9" t="s">
         <v>57</v>
-      </c>
-      <c r="E9" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E10" t="s">
         <v>21</v>
@@ -1782,10 +1809,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1809,10 +1836,10 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>38</v>
+        <v>113</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -1822,12 +1849,8 @@
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>41</v>
-      </c>
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
@@ -1836,8 +1859,12 @@
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
+      <c r="A4" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -1847,7 +1874,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>21</v>
@@ -1860,12 +1887,6 @@
       <c r="H5" s="2"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>20</v>
-      </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -1874,11 +1895,11 @@
       <c r="H6" s="2"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>47</v>
+      <c r="A7" s="3" t="s">
+        <v>44</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>43</v>
+        <v>20</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
@@ -1888,8 +1909,12 @@
       <c r="H7" s="2"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
+      <c r="A8" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>41</v>
+      </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -1898,12 +1923,8 @@
       <c r="H8" s="2"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>20</v>
-      </c>
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
@@ -1913,10 +1934,10 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
@@ -1926,8 +1947,12 @@
       <c r="H10" s="2"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
+      <c r="A11" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
@@ -1974,6 +1999,16 @@
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
(U)    new plan lifts add
</commit_message>
<xml_diff>
--- a/Suppl/Thrive Fitness Plan - Lifting.xlsx
+++ b/Suppl/Thrive Fitness Plan - Lifting.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="72">
   <si>
     <t>Lying Hamstring Curls</t>
   </si>
@@ -226,6 +226,15 @@
   </si>
   <si>
     <t>3x120s</t>
+  </si>
+  <si>
+    <t>Bosu Ball Crunches</t>
+  </si>
+  <si>
+    <t>Selectorized Ab Crunches</t>
+  </si>
+  <si>
+    <t>3x16</t>
   </si>
 </sst>
 </file>
@@ -381,7 +390,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -431,6 +440,9 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -712,10 +724,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L40"/>
+  <dimension ref="A1:L41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1078,12 +1090,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="1"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="11"/>
+    <row r="15" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="10"/>
+      <c r="B15" s="20"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="21"/>
       <c r="F15" s="11"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
@@ -1093,17 +1105,9 @@
       <c r="L15" s="2"/>
     </row>
     <row r="16" spans="1:12" s="2" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="8" t="s">
-        <v>33</v>
-      </c>
+      <c r="A16" s="1"/>
+      <c r="B16" s="14"/>
+      <c r="E16" s="11"/>
       <c r="F16" s="11"/>
       <c r="G16" s="6" t="s">
         <v>25</v>
@@ -1117,15 +1121,17 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="26"/>
-      <c r="B17" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="C17" s="16"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="24" t="s">
-        <v>5</v>
+    <row r="17" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="8" t="s">
+        <v>33</v>
       </c>
       <c r="F17" s="5"/>
       <c r="G17" s="27"/>
@@ -1142,12 +1148,12 @@
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="26"/>
       <c r="B18" s="16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C18" s="16"/>
       <c r="D18" s="16"/>
       <c r="E18" s="24" t="s">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="F18" s="5"/>
       <c r="G18" s="27"/>
@@ -1161,14 +1167,14 @@
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="15"/>
+      <c r="A19" s="26"/>
       <c r="B19" s="16" t="s">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="C19" s="16"/>
       <c r="D19" s="16"/>
       <c r="E19" s="24" t="s">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="F19" s="2"/>
       <c r="G19" s="27"/>
@@ -1184,101 +1190,101 @@
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="15"/>
       <c r="B20" s="16" t="s">
-        <v>46</v>
+        <v>0</v>
       </c>
       <c r="C20" s="16"/>
       <c r="D20" s="16"/>
       <c r="E20" s="24" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F20" s="2"/>
       <c r="G20" s="18"/>
       <c r="H20" s="19" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="I20" s="19"/>
       <c r="J20" s="19"/>
       <c r="K20" s="23" t="s">
-        <v>4</v>
+        <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="26"/>
+      <c r="A21" s="15"/>
       <c r="B21" s="16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C21" s="16"/>
       <c r="D21" s="16"/>
       <c r="E21" s="24" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F21" s="2"/>
       <c r="G21" s="18"/>
       <c r="H21" s="19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I21" s="19"/>
       <c r="J21" s="19"/>
       <c r="K21" s="23" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="26"/>
       <c r="B22" s="16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C22" s="16"/>
       <c r="D22" s="16"/>
       <c r="E22" s="24" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="F22" s="2"/>
       <c r="G22" s="18"/>
       <c r="H22" s="19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I22" s="19"/>
       <c r="J22" s="19"/>
       <c r="K22" s="23" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="26"/>
       <c r="B23" s="16" t="s">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="C23" s="16"/>
       <c r="D23" s="16"/>
       <c r="E23" s="24" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F23" s="2"/>
       <c r="G23" s="27"/>
       <c r="H23" s="19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I23" s="19"/>
       <c r="J23" s="19"/>
       <c r="K23" s="23" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="15"/>
+      <c r="A24" s="26"/>
       <c r="B24" s="16" t="s">
-        <v>49</v>
+        <v>1</v>
       </c>
       <c r="C24" s="16"/>
       <c r="D24" s="16"/>
       <c r="E24" s="24" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F24" s="2"/>
       <c r="G24" s="27"/>
       <c r="H24" s="19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I24" s="19"/>
       <c r="J24" s="19"/>
@@ -1289,28 +1295,28 @@
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="15"/>
       <c r="B25" s="16" t="s">
-        <v>2</v>
+        <v>49</v>
       </c>
       <c r="C25" s="16"/>
       <c r="D25" s="16"/>
       <c r="E25" s="24" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F25" s="2"/>
-      <c r="G25" s="27"/>
+      <c r="G25" s="18"/>
       <c r="H25" s="19" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I25" s="19"/>
       <c r="J25" s="19"/>
       <c r="K25" s="23" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="15"/>
       <c r="B26" s="16" t="s">
-        <v>50</v>
+        <v>2</v>
       </c>
       <c r="C26" s="16"/>
       <c r="D26" s="16"/>
@@ -1318,24 +1324,36 @@
         <v>3</v>
       </c>
       <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
-      <c r="I26" s="2"/>
-      <c r="J26" s="2"/>
-      <c r="K26" s="2"/>
+      <c r="G26" s="18"/>
+      <c r="H26" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="I26" s="19"/>
+      <c r="J26" s="19"/>
+      <c r="K26" s="23" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A27" s="2"/>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
+      <c r="A27" s="15"/>
+      <c r="B27" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="C27" s="16"/>
+      <c r="D27" s="16"/>
+      <c r="E27" s="24" t="s">
+        <v>3</v>
+      </c>
       <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
-      <c r="I27" s="2"/>
-      <c r="J27" s="2"/>
-      <c r="K27" s="2"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="I27" s="18"/>
+      <c r="J27" s="18"/>
+      <c r="K27" s="30" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
@@ -1435,6 +1453,11 @@
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
       <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="2"/>
+      <c r="J35" s="2"/>
+      <c r="K35" s="2"/>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
@@ -1475,6 +1498,13 @@
       <c r="D40" s="2"/>
       <c r="E40" s="2"/>
       <c r="F40" s="2"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" s="2"/>
+      <c r="B41" s="2"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
(+)    plan corrections & diet update
</commit_message>
<xml_diff>
--- a/Suppl/Thrive Fitness Plan - Lifting.xlsx
+++ b/Suppl/Thrive Fitness Plan - Lifting.xlsx
@@ -153,9 +153,6 @@
     <t>Dumbbell Squat-to-Press</t>
   </si>
   <si>
-    <t>Machine Individual Leg Press</t>
-  </si>
-  <si>
     <t>Dumbbell Lunges</t>
   </si>
   <si>
@@ -235,6 +232,9 @@
   </si>
   <si>
     <t>Dumbbell Curls</t>
+  </si>
+  <si>
+    <t>Machine Leg Press</t>
   </si>
 </sst>
 </file>
@@ -727,7 +727,7 @@
   <dimension ref="A1:L41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -914,7 +914,7 @@
       <c r="F6" s="11"/>
       <c r="G6" s="25"/>
       <c r="H6" s="13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I6" s="13"/>
       <c r="J6" s="13"/>
@@ -935,7 +935,7 @@
       <c r="F7" s="11"/>
       <c r="G7" s="25"/>
       <c r="H7" s="13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I7" s="13"/>
       <c r="J7" s="13"/>
@@ -956,12 +956,12 @@
       <c r="F8" s="11"/>
       <c r="G8" s="25"/>
       <c r="H8" s="13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I8" s="13"/>
       <c r="J8" s="13"/>
       <c r="K8" s="22" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -977,7 +977,7 @@
       <c r="F9" s="11"/>
       <c r="G9" s="12"/>
       <c r="H9" s="13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I9" s="13"/>
       <c r="J9" s="13"/>
@@ -998,7 +998,7 @@
       <c r="F10" s="9"/>
       <c r="G10" s="12"/>
       <c r="H10" s="13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I10" s="13"/>
       <c r="J10" s="13"/>
@@ -1030,17 +1030,17 @@
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="10"/>
       <c r="B12" s="20" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C12" s="20"/>
       <c r="D12" s="20"/>
       <c r="E12" s="21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F12" s="11"/>
       <c r="G12" s="25"/>
       <c r="H12" s="13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I12" s="13"/>
       <c r="J12" s="13"/>
@@ -1061,7 +1061,7 @@
       <c r="F13" s="11"/>
       <c r="G13" s="12"/>
       <c r="H13" s="13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I13" s="13"/>
       <c r="J13" s="13"/>
@@ -1082,7 +1082,7 @@
       <c r="F14" s="11"/>
       <c r="G14" s="12"/>
       <c r="H14" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I14" s="13"/>
       <c r="J14" s="13"/>
@@ -1136,7 +1136,7 @@
       <c r="F17" s="5"/>
       <c r="G17" s="27"/>
       <c r="H17" s="19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I17" s="19"/>
       <c r="J17" s="19"/>
@@ -1148,17 +1148,17 @@
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="26"/>
       <c r="B18" s="16" t="s">
-        <v>44</v>
+        <v>71</v>
       </c>
       <c r="C18" s="16"/>
       <c r="D18" s="16"/>
       <c r="E18" s="24" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F18" s="5"/>
       <c r="G18" s="27"/>
       <c r="H18" s="19" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I18" s="19"/>
       <c r="J18" s="19"/>
@@ -1169,7 +1169,7 @@
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="26"/>
       <c r="B19" s="16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C19" s="16"/>
       <c r="D19" s="16"/>
@@ -1179,12 +1179,12 @@
       <c r="F19" s="2"/>
       <c r="G19" s="27"/>
       <c r="H19" s="19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I19" s="19"/>
       <c r="J19" s="19"/>
       <c r="K19" s="23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -1200,18 +1200,18 @@
       <c r="F20" s="2"/>
       <c r="G20" s="18"/>
       <c r="H20" s="19" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I20" s="19"/>
       <c r="J20" s="19"/>
       <c r="K20" s="23" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="15"/>
       <c r="B21" s="16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C21" s="16"/>
       <c r="D21" s="16"/>
@@ -1221,7 +1221,7 @@
       <c r="F21" s="2"/>
       <c r="G21" s="18"/>
       <c r="H21" s="19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I21" s="19"/>
       <c r="J21" s="19"/>
@@ -1232,7 +1232,7 @@
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="26"/>
       <c r="B22" s="16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C22" s="16"/>
       <c r="D22" s="16"/>
@@ -1242,7 +1242,7 @@
       <c r="F22" s="2"/>
       <c r="G22" s="27"/>
       <c r="H22" s="19" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I22" s="19"/>
       <c r="J22" s="19"/>
@@ -1253,7 +1253,7 @@
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="26"/>
       <c r="B23" s="16" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C23" s="16"/>
       <c r="D23" s="16"/>
@@ -1263,7 +1263,7 @@
       <c r="F23" s="2"/>
       <c r="G23" s="27"/>
       <c r="H23" s="19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I23" s="19"/>
       <c r="J23" s="19"/>
@@ -1284,7 +1284,7 @@
       <c r="F24" s="2"/>
       <c r="G24" s="18"/>
       <c r="H24" s="19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I24" s="19"/>
       <c r="J24" s="19"/>
@@ -1295,7 +1295,7 @@
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="15"/>
       <c r="B25" s="16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C25" s="16"/>
       <c r="D25" s="16"/>
@@ -1305,7 +1305,7 @@
       <c r="F25" s="2"/>
       <c r="G25" s="18"/>
       <c r="H25" s="19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I25" s="19"/>
       <c r="J25" s="19"/>
@@ -1326,18 +1326,18 @@
       <c r="F26" s="2"/>
       <c r="G26" s="18"/>
       <c r="H26" s="18" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I26" s="18"/>
       <c r="J26" s="18"/>
       <c r="K26" s="29" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="15"/>
       <c r="B27" s="16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C27" s="16"/>
       <c r="D27" s="16"/>

</xml_diff>